<commit_message>
Backend update - document adder + rest updates
Adding document adder
Adding translate endpoint for restAssistant
Fixing endpoints and methods for restDocuments
Adding new endpoint for restSurvey
Updating excel documents with columns and weights
</commit_message>
<xml_diff>
--- a/iaff_assistant/documents/Citizenship/Polish Citizenship.xlsx
+++ b/iaff_assistant/documents/Citizenship/Polish Citizenship.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ZPI\ZPI_VAF\iaff_assistant\documents\Citizenship\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vano\Documents\GitHub\ZPI_VAF\iaff_assistant\documents\Citizenship\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{982DD0D2-94F0-48BB-88D0-F77ED4AE1A3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41D4A902-74F7-4C1B-B41D-ED3B06557FBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9550" yWindow="0" windowWidth="9740" windowHeight="10170" xr2:uid="{05A09E01-6CEA-49BF-ADF0-F99920407A48}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20760" windowHeight="11175" xr2:uid="{05A09E01-6CEA-49BF-ADF0-F99920407A48}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>Pathways and requirements for obtaining Polish citizenship, including marriage, descent, investment, and naturalization, along with the application process and associated benefits.</t>
   </si>
@@ -147,6 +147,9 @@
   </si>
   <si>
     <t>image</t>
+  </si>
+  <si>
+    <t>citizenship</t>
   </si>
 </sst>
 </file>
@@ -513,18 +516,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D3BBB31-F0CE-4DFD-993C-26209787C84D}">
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.81640625" customWidth="1"/>
-    <col min="2" max="2" width="110.54296875" customWidth="1"/>
-    <col min="3" max="3" width="57.90625" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" customWidth="1"/>
+    <col min="2" max="2" width="110.5703125" customWidth="1"/>
+    <col min="3" max="3" width="57.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -574,7 +577,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -583,6 +586,33 @@
       </c>
       <c r="C2" s="1" t="s">
         <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2">
+        <v>24</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>10</v>
+      </c>
+      <c r="M2">
+        <v>10</v>
+      </c>
+      <c r="N2">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added paths to images in documents
</commit_message>
<xml_diff>
--- a/iaff_assistant/documents/Citizenship/Polish Citizenship.xlsx
+++ b/iaff_assistant/documents/Citizenship/Polish Citizenship.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vano\Documents\GitHub\ZPI_VAF\iaff_assistant\documents\Citizenship\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\STUDIA\ZPI\ZPI_VAF\iaff_assistant\documents\Citizenship\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41D4A902-74F7-4C1B-B41D-ED3B06557FBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01300FA3-21C0-4EFE-B49C-06AEA39FF799}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20760" windowHeight="11175" xr2:uid="{05A09E01-6CEA-49BF-ADF0-F99920407A48}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="13584" windowHeight="8964" xr2:uid="{05A09E01-6CEA-49BF-ADF0-F99920407A48}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>Pathways and requirements for obtaining Polish citizenship, including marriage, descent, investment, and naturalization, along with the application process and associated benefits.</t>
   </si>
@@ -151,6 +151,9 @@
   <si>
     <t>citizenship</t>
   </si>
+  <si>
+    <t>C:Users/vano/Documents/GitHub/ZPI_VAF/iaff_assistant/images/Citizenship/citizenship.jpg</t>
+  </si>
 </sst>
 </file>
 
@@ -202,7 +205,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -218,9 +221,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Pakiet Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -258,7 +261,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Pakiet Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -364,7 +367,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Pakiet Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -516,18 +519,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D3BBB31-F0CE-4DFD-993C-26209787C84D}">
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G2" workbookViewId="0">
       <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" customWidth="1"/>
-    <col min="2" max="2" width="110.5703125" customWidth="1"/>
-    <col min="3" max="3" width="57.85546875" customWidth="1"/>
+    <col min="1" max="1" width="19.88671875" customWidth="1"/>
+    <col min="2" max="2" width="110.5546875" customWidth="1"/>
+    <col min="3" max="3" width="57.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -577,7 +580,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -613,6 +616,9 @@
       </c>
       <c r="N2">
         <v>10</v>
+      </c>
+      <c r="P2" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>